<commit_message>
Add new Testcase in MyLocationTest Class
</commit_message>
<xml_diff>
--- a/com.supermarket/src/main/resource/ExcelFile/TestData.xlsx
+++ b/com.supermarket/src/main/resource/ExcelFile/TestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MINNU\eclipse-workspace\com.supermarket\src\main\resource\ExcelFile\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MINNU\git\TestRepository\com.supermarket\src\main\resource\ExcelFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6903BA24-ADD9-4B9E-8EDD-85393F308486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D459223D-D3D4-4E94-805E-019C2BB8CBC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
   <si>
     <t>username</t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t>lkj</t>
+  </si>
+  <si>
+    <t>locationseach</t>
+  </si>
+  <si>
+    <t>fgh</t>
   </si>
 </sst>
 </file>
@@ -451,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,6 +677,14 @@
         <v>23</v>
       </c>
     </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>